<commit_message>
change chart type from 2 independent data series to one independent-dependent data series
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1738675 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/SimpleScatterChart.xlsx
+++ b/test-data/spreadsheet/SimpleScatterChart.xlsx
@@ -139,6 +139,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -162,22 +173,8 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$1:$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Y</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$B$2</c:f>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -185,60 +182,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$1:$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Y</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$B$3</c:f>
+              <c:f>Sheet1!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
@@ -256,11 +212,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="660799752"/>
-        <c:axId val="660808768"/>
+        <c:axId val="157002856"/>
+        <c:axId val="157003248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="660799752"/>
+        <c:axId val="157002856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -280,6 +236,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -316,12 +273,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="660808768"/>
+        <c:crossAx val="157003248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="660808768"/>
+        <c:axId val="157003248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +335,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="660799752"/>
+        <c:crossAx val="157002856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -474,6 +431,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -512,6 +470,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -535,22 +504,8 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$1:$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Y</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$B$2</c:f>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -558,60 +513,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$1:$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Y</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$B$3</c:f>
+              <c:f>Sheet1!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
@@ -629,11 +543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="660800928"/>
-        <c:axId val="660809944"/>
+        <c:axId val="157004032"/>
+        <c:axId val="346269296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="660800928"/>
+        <c:axId val="157004032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,6 +567,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -689,12 +604,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="660809944"/>
+        <c:crossAx val="346269296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="660809944"/>
+        <c:axId val="346269296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="660800928"/>
+        <c:crossAx val="157004032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -765,6 +680,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>

</xml_diff>